<commit_message>
added national validity check
</commit_message>
<xml_diff>
--- a/Prelim_Data/Arizona_Alluvial/Arizona_Alluvial_30_90.xlsx
+++ b/Prelim_Data/Arizona_Alluvial/Arizona_Alluvial_30_90.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucdavis365-my.sharepoint.com/personal/aahernes_ucdavis_edu/Documents/WORK/DahlkeLab_LAWR/Prelim_Data/Arizona_Alluvial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_DD1D4CC7600C08ACD775E9BA81B9D8C2C7439375" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAD0A5AA-BEE5-492C-8163-EC2BD87477F8}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_DD1D4CC7600C08ACD775E9BA81B9D8C2C7439375" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5EFE70E-723F-4814-8A92-E2C9BBD976FA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="13740" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site_metrics" sheetId="1" r:id="rId1"/>
@@ -1179,10 +1179,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1472,12 +1468,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="Y23" sqref="Y23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" customWidth="1"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>